<commit_message>
add SNR and NTN
</commit_message>
<xml_diff>
--- a/src/test/resources/Complex/KBSklt0508.xlsx
+++ b/src/test/resources/Complex/KBSklt0508.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Project Sources\Autex Webshop Content Manager\src\test\resources\Complex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9430CE05-710E-4866-91A7-B72BE4009289}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DA7EC5-AFAF-43D9-B72E-25F1BCD8DCF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="22140" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20136" yWindow="-12840" windowWidth="20376" windowHeight="12816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -12067,7 +12076,7 @@
   <dimension ref="A1:D3376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>